<commit_message>
Atualiza sistema adicionando funcionalidades
</commit_message>
<xml_diff>
--- a/Reports/database_tables.xlsx
+++ b/Reports/database_tables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="337">
   <si>
     <t>idSala</t>
   </si>
@@ -754,6 +754,195 @@
     <t>2023-07-31</t>
   </si>
   <si>
+    <t>2023-07-24</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>2023-07-27</t>
+  </si>
+  <si>
+    <t>2023-08-03</t>
+  </si>
+  <si>
+    <t>2023-08-07</t>
+  </si>
+  <si>
+    <t>2023-08-10</t>
+  </si>
+  <si>
+    <t>2023-08-14</t>
+  </si>
+  <si>
+    <t>2023-08-17</t>
+  </si>
+  <si>
+    <t>2023-08-21</t>
+  </si>
+  <si>
+    <t>2023-08-24</t>
+  </si>
+  <si>
+    <t>2023-08-28</t>
+  </si>
+  <si>
+    <t>2023-08-31</t>
+  </si>
+  <si>
+    <t>2023-09-04</t>
+  </si>
+  <si>
+    <t>2023-09-07</t>
+  </si>
+  <si>
+    <t>2023-09-11</t>
+  </si>
+  <si>
+    <t>2023-09-14</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>19:00:00</t>
+  </si>
+  <si>
+    <t>22:00:00</t>
+  </si>
+  <si>
+    <t>2023-02-04</t>
+  </si>
+  <si>
+    <t>09:00:00</t>
+  </si>
+  <si>
+    <t>2023-02-11</t>
+  </si>
+  <si>
+    <t>2023-02-18</t>
+  </si>
+  <si>
+    <t>2023-02-25</t>
+  </si>
+  <si>
+    <t>2023-03-04</t>
+  </si>
+  <si>
+    <t>2023-03-11</t>
+  </si>
+  <si>
+    <t>2023-03-18</t>
+  </si>
+  <si>
+    <t>2023-03-25</t>
+  </si>
+  <si>
+    <t>2023-04-01</t>
+  </si>
+  <si>
+    <t>2023-04-08</t>
+  </si>
+  <si>
+    <t>2023-04-15</t>
+  </si>
+  <si>
+    <t>2023-04-22</t>
+  </si>
+  <si>
+    <t>2023-04-29</t>
+  </si>
+  <si>
+    <t>2023-05-06</t>
+  </si>
+  <si>
+    <t>2023-05-13</t>
+  </si>
+  <si>
+    <t>2023-05-20</t>
+  </si>
+  <si>
+    <t>2023-05-27</t>
+  </si>
+  <si>
+    <t>2023-06-03</t>
+  </si>
+  <si>
+    <t>2023-06-10</t>
+  </si>
+  <si>
+    <t>2023-06-17</t>
+  </si>
+  <si>
+    <t>2023-06-24</t>
+  </si>
+  <si>
+    <t>2023-07-01</t>
+  </si>
+  <si>
+    <t>2023-07-08</t>
+  </si>
+  <si>
+    <t>2023-07-15</t>
+  </si>
+  <si>
+    <t>2023-07-22</t>
+  </si>
+  <si>
+    <t>2023-07-29</t>
+  </si>
+  <si>
+    <t>2023-08-05</t>
+  </si>
+  <si>
+    <t>2023-08-12</t>
+  </si>
+  <si>
+    <t>2023-08-19</t>
+  </si>
+  <si>
+    <t>2023-08-26</t>
+  </si>
+  <si>
+    <t>2023-09-02</t>
+  </si>
+  <si>
+    <t>2023-09-09</t>
+  </si>
+  <si>
+    <t>2023-09-16</t>
+  </si>
+  <si>
+    <t>2023-09-23</t>
+  </si>
+  <si>
+    <t>2023-09-30</t>
+  </si>
+  <si>
+    <t>2023-10-07</t>
+  </si>
+  <si>
+    <t>2023-10-14</t>
+  </si>
+  <si>
+    <t>2023-10-21</t>
+  </si>
+  <si>
+    <t>2023-10-28</t>
+  </si>
+  <si>
+    <t>2023-11-04</t>
+  </si>
+  <si>
+    <t>2023-11-11</t>
+  </si>
+  <si>
     <t>idDocenteResponsavel</t>
   </si>
   <si>
@@ -772,12 +961,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>2023-02-04</t>
-  </si>
-  <si>
-    <t>2023-11-11</t>
-  </si>
-  <si>
     <t>em andamento</t>
   </si>
   <si>
@@ -793,12 +976,6 @@
     <t>FBEPL90231</t>
   </si>
   <si>
-    <t>2023-07-22</t>
-  </si>
-  <si>
-    <t>2023-09-23</t>
-  </si>
-  <si>
     <t>FBEPL90232</t>
   </si>
   <si>
@@ -830,9 +1007,6 @@
   </si>
   <si>
     <t>FBEPWBI238</t>
-  </si>
-  <si>
-    <t>2023-08-17</t>
   </si>
   <si>
     <t>FBEPWBI236</t>
@@ -2947,7 +3121,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3013,6 +3187,1226 @@
       </c>
       <c r="F3">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>511</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>512</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>513</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>514</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>515</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>516</v>
+      </c>
+      <c r="B9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>517</v>
+      </c>
+      <c r="B10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>518</v>
+      </c>
+      <c r="B11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>519</v>
+      </c>
+      <c r="B12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>520</v>
+      </c>
+      <c r="B13" t="s">
+        <v>252</v>
+      </c>
+      <c r="C13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" t="s">
+        <v>244</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>521</v>
+      </c>
+      <c r="B14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>522</v>
+      </c>
+      <c r="B15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>523</v>
+      </c>
+      <c r="B16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" t="s">
+        <v>244</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>524</v>
+      </c>
+      <c r="B17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>525</v>
+      </c>
+      <c r="B18" t="s">
+        <v>257</v>
+      </c>
+      <c r="C18" t="s">
+        <v>243</v>
+      </c>
+      <c r="D18" t="s">
+        <v>244</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>526</v>
+      </c>
+      <c r="B19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D19" t="s">
+        <v>244</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>527</v>
+      </c>
+      <c r="B20" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" t="s">
+        <v>243</v>
+      </c>
+      <c r="D20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>528</v>
+      </c>
+      <c r="B21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D21" t="s">
+        <v>244</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>529</v>
+      </c>
+      <c r="B22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>530</v>
+      </c>
+      <c r="B23" t="s">
+        <v>245</v>
+      </c>
+      <c r="C23" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" t="s">
+        <v>262</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>531</v>
+      </c>
+      <c r="B24" t="s">
+        <v>263</v>
+      </c>
+      <c r="C24" t="s">
+        <v>210</v>
+      </c>
+      <c r="D24" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>532</v>
+      </c>
+      <c r="B25" t="s">
+        <v>265</v>
+      </c>
+      <c r="C25" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" t="s">
+        <v>264</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>533</v>
+      </c>
+      <c r="B26" t="s">
+        <v>266</v>
+      </c>
+      <c r="C26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" t="s">
+        <v>264</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>534</v>
+      </c>
+      <c r="B27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" t="s">
+        <v>264</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>535</v>
+      </c>
+      <c r="B28" t="s">
+        <v>268</v>
+      </c>
+      <c r="C28" t="s">
+        <v>210</v>
+      </c>
+      <c r="D28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>536</v>
+      </c>
+      <c r="B29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C29" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" t="s">
+        <v>264</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>537</v>
+      </c>
+      <c r="B30" t="s">
+        <v>270</v>
+      </c>
+      <c r="C30" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" t="s">
+        <v>264</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>538</v>
+      </c>
+      <c r="B31" t="s">
+        <v>271</v>
+      </c>
+      <c r="C31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D31" t="s">
+        <v>264</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>539</v>
+      </c>
+      <c r="B32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D32" t="s">
+        <v>264</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>540</v>
+      </c>
+      <c r="B33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33" t="s">
+        <v>210</v>
+      </c>
+      <c r="D33" t="s">
+        <v>264</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>541</v>
+      </c>
+      <c r="B34" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" t="s">
+        <v>210</v>
+      </c>
+      <c r="D34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>542</v>
+      </c>
+      <c r="B35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C35" t="s">
+        <v>210</v>
+      </c>
+      <c r="D35" t="s">
+        <v>264</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>543</v>
+      </c>
+      <c r="B36" t="s">
+        <v>276</v>
+      </c>
+      <c r="C36" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36" t="s">
+        <v>264</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>544</v>
+      </c>
+      <c r="B37" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" t="s">
+        <v>264</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>545</v>
+      </c>
+      <c r="B38" t="s">
+        <v>278</v>
+      </c>
+      <c r="C38" t="s">
+        <v>210</v>
+      </c>
+      <c r="D38" t="s">
+        <v>264</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>546</v>
+      </c>
+      <c r="B39" t="s">
+        <v>279</v>
+      </c>
+      <c r="C39" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>547</v>
+      </c>
+      <c r="B40" t="s">
+        <v>280</v>
+      </c>
+      <c r="C40" t="s">
+        <v>210</v>
+      </c>
+      <c r="D40" t="s">
+        <v>264</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>548</v>
+      </c>
+      <c r="B41" t="s">
+        <v>281</v>
+      </c>
+      <c r="C41" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" t="s">
+        <v>264</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>549</v>
+      </c>
+      <c r="B42" t="s">
+        <v>282</v>
+      </c>
+      <c r="C42" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42" t="s">
+        <v>264</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>550</v>
+      </c>
+      <c r="B43" t="s">
+        <v>283</v>
+      </c>
+      <c r="C43" t="s">
+        <v>210</v>
+      </c>
+      <c r="D43" t="s">
+        <v>264</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>551</v>
+      </c>
+      <c r="B44" t="s">
+        <v>284</v>
+      </c>
+      <c r="C44" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" t="s">
+        <v>264</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>552</v>
+      </c>
+      <c r="B45" t="s">
+        <v>285</v>
+      </c>
+      <c r="C45" t="s">
+        <v>210</v>
+      </c>
+      <c r="D45" t="s">
+        <v>264</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>553</v>
+      </c>
+      <c r="B46" t="s">
+        <v>286</v>
+      </c>
+      <c r="C46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D46" t="s">
+        <v>264</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>554</v>
+      </c>
+      <c r="B47" t="s">
+        <v>287</v>
+      </c>
+      <c r="C47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D47" t="s">
+        <v>264</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>555</v>
+      </c>
+      <c r="B48" t="s">
+        <v>288</v>
+      </c>
+      <c r="C48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D48" t="s">
+        <v>264</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>556</v>
+      </c>
+      <c r="B49" t="s">
+        <v>289</v>
+      </c>
+      <c r="C49" t="s">
+        <v>210</v>
+      </c>
+      <c r="D49" t="s">
+        <v>264</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>557</v>
+      </c>
+      <c r="B50" t="s">
+        <v>290</v>
+      </c>
+      <c r="C50" t="s">
+        <v>210</v>
+      </c>
+      <c r="D50" t="s">
+        <v>264</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>558</v>
+      </c>
+      <c r="B51" t="s">
+        <v>291</v>
+      </c>
+      <c r="C51" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" t="s">
+        <v>264</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>559</v>
+      </c>
+      <c r="B52" t="s">
+        <v>292</v>
+      </c>
+      <c r="C52" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" t="s">
+        <v>264</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>560</v>
+      </c>
+      <c r="B53" t="s">
+        <v>293</v>
+      </c>
+      <c r="C53" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" t="s">
+        <v>264</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>561</v>
+      </c>
+      <c r="B54" t="s">
+        <v>294</v>
+      </c>
+      <c r="C54" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" t="s">
+        <v>264</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>562</v>
+      </c>
+      <c r="B55" t="s">
+        <v>295</v>
+      </c>
+      <c r="C55" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" t="s">
+        <v>264</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>563</v>
+      </c>
+      <c r="B56" t="s">
+        <v>296</v>
+      </c>
+      <c r="C56" t="s">
+        <v>210</v>
+      </c>
+      <c r="D56" t="s">
+        <v>264</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>564</v>
+      </c>
+      <c r="B57" t="s">
+        <v>297</v>
+      </c>
+      <c r="C57" t="s">
+        <v>210</v>
+      </c>
+      <c r="D57" t="s">
+        <v>264</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>565</v>
+      </c>
+      <c r="B58" t="s">
+        <v>298</v>
+      </c>
+      <c r="C58" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" t="s">
+        <v>264</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>566</v>
+      </c>
+      <c r="B59" t="s">
+        <v>299</v>
+      </c>
+      <c r="C59" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" t="s">
+        <v>264</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>567</v>
+      </c>
+      <c r="B60" t="s">
+        <v>300</v>
+      </c>
+      <c r="C60" t="s">
+        <v>210</v>
+      </c>
+      <c r="D60" t="s">
+        <v>264</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>568</v>
+      </c>
+      <c r="B61" t="s">
+        <v>301</v>
+      </c>
+      <c r="C61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" t="s">
+        <v>264</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>569</v>
+      </c>
+      <c r="B62" t="s">
+        <v>302</v>
+      </c>
+      <c r="C62" t="s">
+        <v>210</v>
+      </c>
+      <c r="D62" t="s">
+        <v>264</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>570</v>
+      </c>
+      <c r="B63" t="s">
+        <v>303</v>
+      </c>
+      <c r="C63" t="s">
+        <v>210</v>
+      </c>
+      <c r="D63" t="s">
+        <v>264</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>571</v>
+      </c>
+      <c r="B64" t="s">
+        <v>304</v>
+      </c>
+      <c r="C64" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" t="s">
+        <v>264</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3053,22 +4447,22 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>305</v>
       </c>
       <c r="D1" t="s">
         <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>243</v>
+        <v>306</v>
       </c>
       <c r="F1" t="s">
-        <v>244</v>
+        <v>307</v>
       </c>
       <c r="G1" t="s">
-        <v>245</v>
+        <v>308</v>
       </c>
       <c r="H1" t="s">
-        <v>246</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3076,7 +4470,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="C2">
         <v>1085900</v>
@@ -3088,13 +4482,13 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="G2" t="s">
-        <v>249</v>
+        <v>304</v>
       </c>
       <c r="H2" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3102,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="C3">
         <v>1085900</v>
@@ -3114,13 +4508,13 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>252</v>
+        <v>313</v>
       </c>
       <c r="G3" t="s">
-        <v>253</v>
+        <v>314</v>
       </c>
       <c r="H3" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3128,7 +4522,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>315</v>
       </c>
       <c r="C4">
         <v>1085905</v>
@@ -3140,13 +4534,13 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>288</v>
       </c>
       <c r="G4" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="H4" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3154,7 +4548,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>316</v>
       </c>
       <c r="C5">
         <v>1085905</v>
@@ -3166,13 +4560,13 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>317</v>
       </c>
       <c r="G5" t="s">
-        <v>259</v>
+        <v>318</v>
       </c>
       <c r="H5" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3180,7 +4574,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>320</v>
       </c>
       <c r="C6">
         <v>1085905</v>
@@ -3192,13 +4586,13 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>262</v>
+        <v>321</v>
       </c>
       <c r="G6" t="s">
-        <v>263</v>
+        <v>322</v>
       </c>
       <c r="H6" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3206,7 +4600,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>323</v>
       </c>
       <c r="C7">
         <v>1085909</v>
@@ -3218,10 +4612,10 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>265</v>
+        <v>324</v>
       </c>
       <c r="G7" t="s">
-        <v>266</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3229,7 +4623,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>326</v>
       </c>
       <c r="C8">
         <v>1085899</v>
@@ -3241,13 +4635,13 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>265</v>
+        <v>324</v>
       </c>
       <c r="G8" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="H8" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3255,7 +4649,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>327</v>
       </c>
       <c r="C9">
         <v>1085899</v>
@@ -3267,13 +4661,13 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>270</v>
+        <v>328</v>
       </c>
       <c r="G9" t="s">
-        <v>271</v>
+        <v>329</v>
       </c>
       <c r="H9" t="s">
-        <v>272</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3281,7 +4675,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>331</v>
       </c>
       <c r="C10">
         <v>1085903</v>
@@ -3293,13 +4687,13 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>274</v>
+        <v>332</v>
       </c>
       <c r="G10" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="H10" t="s">
-        <v>276</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3307,7 +4701,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>335</v>
       </c>
       <c r="C11">
         <v>1085909</v>
@@ -3319,13 +4713,13 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>278</v>
+        <v>336</v>
       </c>
       <c r="G11" t="s">
-        <v>249</v>
+        <v>304</v>
       </c>
       <c r="H11" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>